<commit_message>
incluindo DTB - IBGE
</commit_message>
<xml_diff>
--- a/Bot-Varredura/dominios.xlsx
+++ b/Bot-Varredura/dominios.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">DATA EXTRACAO</t>
   </si>
   <si>
-    <t xml:space="preserve">angra.rj.gov.br</t>
+    <t xml:space="preserve">coloque_o_dominio_aqui</t>
   </si>
 </sst>
 </file>
@@ -121,12 +121,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,30 +151,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:C2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.51"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>